<commit_message>
started µ's in function
</commit_message>
<xml_diff>
--- a/Excel_Files/Stats_Populations/2.5_cm/673_nm_s.xlsx
+++ b/Excel_Files/Stats_Populations/2.5_cm/673_nm_s.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/braulio/Documents/BCH_Harvard/Code/Diffuse_Reflectance/Diffuse_Reflectance_Analysis/Excel_Files/Stats_Populations/2.5_cm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E0C282-1D89-EB44-BD19-9F927EAC5B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="21260" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -202,8 +208,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,16 +225,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria Math"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -237,17 +262,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -255,10 +285,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -266,13 +326,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -310,7 +378,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -344,6 +412,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -378,9 +447,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,231 +623,230 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" style="1"/>
+    <col min="2" max="2" width="15.83203125" style="2"/>
+    <col min="3" max="16384" width="15.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" s="7" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" s="7" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J6" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:10" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" s="5" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>